<commit_message>
Fix typos in ERF function description
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/ERF.xlsx
+++ b/xlsx/tests/docs/ERF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BB8C42-570C-48EE-AFDE-E8F4D179760E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED2AEE-287B-4261-AC46-EAC13849AF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BC44EA43-B61B-417F-9ADF-F059B85B51E3}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>ERF(X, Y)</t>
-  </si>
-  <si>
     <t>Formula</t>
   </si>
   <si>
@@ -70,14 +67,17 @@
   <si>
     <t>Unable to convert argument to a number.</t>
   </si>
+  <si>
+    <t>ERF(X,Y)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -124,10 +124,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC17462-0B08-4BD1-9C6A-0FDADCE81763}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +857,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>2</v>
@@ -871,12 +871,12 @@
         <v>0.5</v>
       </c>
       <c r="C25" s="3">
-        <f>ERF(A25, B25)</f>
+        <f>ERF(A25,B25)</f>
         <v>0.52049987781304652</v>
       </c>
       <c r="D25" s="1" t="str">
         <f ca="1">_xlfn.FORMULATEXT(C25)</f>
-        <v>=ERF(A25, B25)</v>
+        <v>=ERF(A25,B25)</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,12 +889,12 @@
         <v>0</v>
       </c>
       <c r="C26" s="3">
-        <f>ERF(A26, B26)</f>
+        <f>ERF(A26,B26)</f>
         <v>-0.52049987781304652</v>
       </c>
       <c r="D26" s="1" t="str">
         <f ca="1">_xlfn.FORMULATEXT(C26)</f>
-        <v>=ERF(A26, B26)</v>
+        <v>=ERF(A26,B26)</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,13 +967,13 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
         <v>=ERF(SQRT(-1))</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -999,7 +999,7 @@
         <v>=ERF("str")</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
         <v>=ERF(10/0)</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>